<commit_message>
Shipping info for INTL
</commit_message>
<xml_diff>
--- a/docs/IMR-AmpliconSubmissionSheet(your_last_name_here).xlsx
+++ b/docs/IMR-AmpliconSubmissionSheet(your_last_name_here).xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="49">
   <si>
     <t xml:space="preserve">Plate 1 </t>
   </si>
@@ -77,9 +77,6 @@
     <t>IMR Sample Requirements:</t>
   </si>
   <si>
-    <t>Clean DNA at &gt;1 ng/uL, 5 uL of each sample in V-bottom PCR plates.</t>
-  </si>
-  <si>
     <t>Instructions:</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
     <t>4. Hand-deliver or ship your plates to the IMR - DNA is relatively stable once purified, so you do not need to use dry ice, but can use regular water-tight ice packs. Make sure to seal the plates in zip-lock bags to prevent them from getting wet.</t>
   </si>
   <si>
-    <t>Integrated Microbiome Resource (IMR) Submission Template v.1 (July 2015)</t>
-  </si>
-  <si>
     <t>Sample1</t>
   </si>
   <si>
@@ -159,13 +153,69 @@
   </si>
   <si>
     <t>Internal Use Only</t>
+  </si>
+  <si>
+    <t>Integrated Microbiome Resource (IMR) Submission Template v.2 (Oct 2015)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FOR INTERNATIONAL SHIPMENTS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> You must declare a commercial value of $1 for Canada Customs and include (preferrentially in additional address line) the following account to cover customs charges: "Dalhousie grant# for customs charges: DAL69318"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clean DNA at &gt;1 ng/uL (preferrably closer to 10 ng/uL), 5 uL of each sample in V-bottom PCR plates (small numbers of samples can be in PCR strips). </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Exception:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> If submitting for multiple domains (16S+18S) or Archaea, send 10 uL ea.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +249,14 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -429,18 +487,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -459,47 +538,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -810,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF50"/>
+  <dimension ref="A1:AF52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,30 +880,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
+      <c r="A1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
       <c r="V1" s="30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="W1" s="30"/>
       <c r="X1" s="30"/>
-      <c r="Y1" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="33"/>
+      <c r="Y1" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="29"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S2" s="7"/>
@@ -864,36 +922,35 @@
       <c r="AF2" s="7"/>
     </row>
     <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="29"/>
-      <c r="I3" s="13" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
+      <c r="J3" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="24"/>
-      <c r="Z3" s="24"/>
-      <c r="AA3" s="24"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="15"/>
+      <c r="AA3" s="15"/>
       <c r="AB3" s="6"/>
       <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
@@ -901,36 +958,35 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="29"/>
-      <c r="I4" s="23" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="19"/>
+      <c r="J4" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24"/>
-      <c r="T4" s="24"/>
-      <c r="U4" s="24"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="24"/>
-      <c r="X4" s="24"/>
-      <c r="Y4" s="24"/>
-      <c r="Z4" s="24"/>
-      <c r="AA4" s="24"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="15"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
@@ -939,22 +995,21 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I5"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
-      <c r="S5" s="24"/>
-      <c r="T5" s="24"/>
-      <c r="U5" s="24"/>
-      <c r="V5" s="24"/>
-      <c r="W5" s="24"/>
-      <c r="X5" s="24"/>
-      <c r="Y5" s="24"/>
-      <c r="Z5" s="24"/>
-      <c r="AA5" s="24"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
       <c r="AB5" s="6"/>
       <c r="AC5" s="6"/>
       <c r="AD5" s="6"/>
@@ -962,31 +1017,30 @@
       <c r="AF5" s="7"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="29"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="24"/>
-      <c r="X6" s="24"/>
-      <c r="Y6" s="24"/>
-      <c r="Z6" s="24"/>
-      <c r="AA6" s="24"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
       <c r="AB6" s="7"/>
       <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
@@ -994,31 +1048,30 @@
       <c r="AF6" s="7"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="29"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
-      <c r="S7" s="24"/>
-      <c r="T7" s="24"/>
-      <c r="U7" s="24"/>
-      <c r="V7" s="24"/>
-      <c r="W7" s="24"/>
-      <c r="X7" s="24"/>
-      <c r="Y7" s="24"/>
-      <c r="Z7" s="24"/>
-      <c r="AA7" s="24"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="19"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="15"/>
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
       <c r="AD7" s="7"/>
@@ -1026,22 +1079,21 @@
       <c r="AF7" s="7"/>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="24"/>
-      <c r="U8" s="24"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="24"/>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="24"/>
-      <c r="AA8" s="24"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+      <c r="AA8" s="15"/>
       <c r="AB8" s="7"/>
       <c r="AC8" s="7"/>
       <c r="AD8" s="7"/>
@@ -1049,333 +1101,279 @@
       <c r="AF8" s="7"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
-      <c r="T9" s="24"/>
-      <c r="U9" s="24"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="24"/>
-      <c r="X9" s="24"/>
-      <c r="Y9" s="24"/>
-      <c r="Z9" s="24"/>
-      <c r="AA9" s="24"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="15"/>
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
       <c r="AE9" s="7"/>
       <c r="AF9" s="7"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+    <row r="10" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="24"/>
-      <c r="S10" s="24"/>
-      <c r="T10" s="24"/>
-      <c r="U10" s="24"/>
-      <c r="V10" s="24"/>
-      <c r="W10" s="24"/>
-      <c r="X10" s="24"/>
-      <c r="Y10" s="24"/>
-      <c r="Z10" s="24"/>
-      <c r="AA10" s="24"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
+      <c r="AA10" s="15"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="11"/>
-      <c r="AA11" s="11"/>
-    </row>
-    <row r="12" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="15"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="15"/>
+      <c r="Y12" s="15"/>
+      <c r="Z12" s="15"/>
+      <c r="AA12" s="15"/>
+    </row>
+    <row r="13" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
-      <c r="T13" s="15"/>
-      <c r="U13" s="15"/>
-      <c r="V13" s="15"/>
-      <c r="W13" s="15"/>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="15"/>
-      <c r="Z13" s="15"/>
-      <c r="AA13" s="16"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
-      <c r="Z14" s="18"/>
-      <c r="AA14" s="19"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="22"/>
+      <c r="U14" s="22"/>
+      <c r="V14" s="22"/>
+      <c r="W14" s="22"/>
+      <c r="X14" s="22"/>
+      <c r="Y14" s="22"/>
+      <c r="Z14" s="22"/>
+      <c r="AA14" s="23"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
-      <c r="C15" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18"/>
-      <c r="V15" s="18"/>
-      <c r="W15" s="18"/>
-      <c r="X15" s="18"/>
-      <c r="Y15" s="18"/>
-      <c r="Z15" s="18"/>
-      <c r="AA15" s="19"/>
-    </row>
-    <row r="16" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="25"/>
+      <c r="V15" s="25"/>
+      <c r="W15" s="25"/>
+      <c r="X15" s="25"/>
+      <c r="Y15" s="25"/>
+      <c r="Z15" s="25"/>
+      <c r="AA15" s="26"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21"/>
-      <c r="S16" s="21"/>
-      <c r="T16" s="21"/>
-      <c r="U16" s="21"/>
-      <c r="V16" s="21"/>
-      <c r="W16" s="21"/>
-      <c r="X16" s="21"/>
-      <c r="Y16" s="21"/>
-      <c r="Z16" s="21"/>
-      <c r="AA16" s="22"/>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="O18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
-      <c r="Z18" s="3"/>
-      <c r="AA18" s="3"/>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="1">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1">
-        <v>2</v>
-      </c>
-      <c r="D19" s="1">
-        <v>3</v>
-      </c>
-      <c r="E19" s="1">
-        <v>4</v>
-      </c>
-      <c r="F19" s="1">
-        <v>5</v>
-      </c>
-      <c r="G19" s="1">
-        <v>6</v>
-      </c>
-      <c r="H19" s="1">
-        <v>7</v>
-      </c>
-      <c r="I19" s="1">
-        <v>8</v>
-      </c>
-      <c r="J19" s="1">
-        <v>9</v>
-      </c>
-      <c r="K19" s="1">
-        <v>10</v>
-      </c>
-      <c r="L19" s="1">
-        <v>11</v>
-      </c>
-      <c r="M19" s="1">
-        <v>12</v>
-      </c>
-      <c r="O19" s="2"/>
-      <c r="P19" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="1">
-        <v>2</v>
-      </c>
-      <c r="R19" s="1">
-        <v>3</v>
-      </c>
-      <c r="S19" s="1">
-        <v>4</v>
-      </c>
-      <c r="T19" s="1">
-        <v>5</v>
-      </c>
-      <c r="U19" s="1">
-        <v>6</v>
-      </c>
-      <c r="V19" s="1">
-        <v>7</v>
-      </c>
-      <c r="W19" s="1">
-        <v>8</v>
-      </c>
-      <c r="X19" s="1">
-        <v>9</v>
-      </c>
-      <c r="Y19" s="1">
-        <v>10</v>
-      </c>
-      <c r="Z19" s="1">
-        <v>11</v>
-      </c>
-      <c r="AA19" s="1">
-        <v>12</v>
-      </c>
+      <c r="C16" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+      <c r="T16" s="25"/>
+      <c r="U16" s="25"/>
+      <c r="V16" s="25"/>
+      <c r="W16" s="25"/>
+      <c r="X16" s="25"/>
+      <c r="Y16" s="25"/>
+      <c r="Z16" s="25"/>
+      <c r="AA16" s="26"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="25"/>
+      <c r="V17" s="25"/>
+      <c r="W17" s="25"/>
+      <c r="X17" s="25"/>
+      <c r="Y17" s="25"/>
+      <c r="Z17" s="25"/>
+      <c r="AA17" s="26"/>
+    </row>
+    <row r="18" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="12"/>
+      <c r="X18" s="12"/>
+      <c r="Y18" s="12"/>
+      <c r="Z18" s="12"/>
+      <c r="AA18" s="13"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>34</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1387,11 +1385,9 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="O20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P20" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
@@ -1405,52 +1401,90 @@
       <c r="AA20" s="3"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2"/>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
         <v>2</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="O21" s="1" t="s">
+      <c r="D21" s="1">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1">
+        <v>7</v>
+      </c>
+      <c r="I21" s="1">
+        <v>8</v>
+      </c>
+      <c r="J21" s="1">
+        <v>9</v>
+      </c>
+      <c r="K21" s="1">
+        <v>10</v>
+      </c>
+      <c r="L21" s="1">
+        <v>11</v>
+      </c>
+      <c r="M21" s="1">
+        <v>12</v>
+      </c>
+      <c r="O21" s="2"/>
+      <c r="P21" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="1">
         <v>2</v>
       </c>
-      <c r="P21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
-      <c r="Z21" s="3"/>
-      <c r="AA21" s="3"/>
+      <c r="R21" s="1">
+        <v>3</v>
+      </c>
+      <c r="S21" s="1">
+        <v>4</v>
+      </c>
+      <c r="T21" s="1">
+        <v>5</v>
+      </c>
+      <c r="U21" s="1">
+        <v>6</v>
+      </c>
+      <c r="V21" s="1">
+        <v>7</v>
+      </c>
+      <c r="W21" s="1">
+        <v>8</v>
+      </c>
+      <c r="X21" s="1">
+        <v>9</v>
+      </c>
+      <c r="Y21" s="1">
+        <v>10</v>
+      </c>
+      <c r="Z21" s="1">
+        <v>11</v>
+      </c>
+      <c r="AA21" s="1">
+        <v>12</v>
+      </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -1463,10 +1497,10 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="O22" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
@@ -1482,13 +1516,13 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -1499,14 +1533,12 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="3" t="s">
+      <c r="M23" s="3"/>
+      <c r="O23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P23" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P23" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
@@ -1522,12 +1554,14 @@
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1537,14 +1571,12 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="M24" s="3"/>
       <c r="O24" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
@@ -1560,12 +1592,14 @@
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1576,12 +1610,14 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P25" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
@@ -1596,10 +1632,10 @@
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1612,12 +1648,14 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P26" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
       <c r="S26" s="3"/>
@@ -1632,10 +1670,10 @@
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1647,11 +1685,11 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="5" t="s">
-        <v>9</v>
+      <c r="M27" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
@@ -1664,12 +1702,15 @@
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
-      <c r="AA27" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="AA27" s="3"/>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -1680,12 +1721,65 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
+      <c r="M28" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A30" s="1"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -1697,103 +1791,11 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
-      <c r="O30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="3"/>
-      <c r="S30" s="3"/>
-      <c r="T30" s="3"/>
-      <c r="U30" s="3"/>
-      <c r="V30" s="3"/>
-      <c r="W30" s="3"/>
-      <c r="X30" s="3"/>
-      <c r="Y30" s="3"/>
-      <c r="Z30" s="3"/>
-      <c r="AA30" s="3"/>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="1">
-        <v>1</v>
-      </c>
-      <c r="C31" s="1">
-        <v>2</v>
-      </c>
-      <c r="D31" s="1">
-        <v>3</v>
-      </c>
-      <c r="E31" s="1">
-        <v>4</v>
-      </c>
-      <c r="F31" s="1">
-        <v>5</v>
-      </c>
-      <c r="G31" s="1">
-        <v>6</v>
-      </c>
-      <c r="H31" s="1">
-        <v>7</v>
-      </c>
-      <c r="I31" s="1">
-        <v>8</v>
-      </c>
-      <c r="J31" s="1">
-        <v>9</v>
-      </c>
-      <c r="K31" s="1">
-        <v>10</v>
-      </c>
-      <c r="L31" s="1">
-        <v>11</v>
-      </c>
-      <c r="M31" s="1">
-        <v>12</v>
-      </c>
-      <c r="O31" s="2"/>
-      <c r="P31" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q31" s="1">
-        <v>2</v>
-      </c>
-      <c r="R31" s="1">
-        <v>3</v>
-      </c>
-      <c r="S31" s="1">
-        <v>4</v>
-      </c>
-      <c r="T31" s="1">
-        <v>5</v>
-      </c>
-      <c r="U31" s="1">
-        <v>6</v>
-      </c>
-      <c r="V31" s="1">
-        <v>7</v>
-      </c>
-      <c r="W31" s="1">
-        <v>8</v>
-      </c>
-      <c r="X31" s="1">
-        <v>9</v>
-      </c>
-      <c r="Y31" s="1">
-        <v>10</v>
-      </c>
-      <c r="Z31" s="1">
-        <v>11</v>
-      </c>
-      <c r="AA31" s="1">
-        <v>12</v>
-      </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="3"/>
+        <v>11</v>
+      </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -1806,7 +1808,7 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
       <c r="O32" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
@@ -1822,40 +1824,84 @@
       <c r="AA32" s="3"/>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="2"/>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1">
         <v>2</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="O33" s="1" t="s">
+      <c r="D33" s="1">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1">
+        <v>4</v>
+      </c>
+      <c r="F33" s="1">
+        <v>5</v>
+      </c>
+      <c r="G33" s="1">
+        <v>6</v>
+      </c>
+      <c r="H33" s="1">
+        <v>7</v>
+      </c>
+      <c r="I33" s="1">
+        <v>8</v>
+      </c>
+      <c r="J33" s="1">
+        <v>9</v>
+      </c>
+      <c r="K33" s="1">
+        <v>10</v>
+      </c>
+      <c r="L33" s="1">
+        <v>11</v>
+      </c>
+      <c r="M33" s="1">
+        <v>12</v>
+      </c>
+      <c r="O33" s="2"/>
+      <c r="P33" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="1">
         <v>2</v>
       </c>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="3"/>
-      <c r="S33" s="3"/>
-      <c r="T33" s="3"/>
-      <c r="U33" s="3"/>
-      <c r="V33" s="3"/>
-      <c r="W33" s="3"/>
-      <c r="X33" s="3"/>
-      <c r="Y33" s="3"/>
-      <c r="Z33" s="3"/>
-      <c r="AA33" s="3"/>
+      <c r="R33" s="1">
+        <v>3</v>
+      </c>
+      <c r="S33" s="1">
+        <v>4</v>
+      </c>
+      <c r="T33" s="1">
+        <v>5</v>
+      </c>
+      <c r="U33" s="1">
+        <v>6</v>
+      </c>
+      <c r="V33" s="1">
+        <v>7</v>
+      </c>
+      <c r="W33" s="1">
+        <v>8</v>
+      </c>
+      <c r="X33" s="1">
+        <v>9</v>
+      </c>
+      <c r="Y33" s="1">
+        <v>10</v>
+      </c>
+      <c r="Z33" s="1">
+        <v>11</v>
+      </c>
+      <c r="AA33" s="1">
+        <v>12</v>
+      </c>
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1870,7 +1916,7 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="O34" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
@@ -1887,7 +1933,7 @@
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1902,7 +1948,7 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="O35" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P35" s="3"/>
       <c r="Q35" s="3"/>
@@ -1919,7 +1965,7 @@
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1934,7 +1980,7 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="O36" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
@@ -1951,7 +1997,7 @@
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1966,7 +2012,7 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="O37" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P37" s="3"/>
       <c r="Q37" s="3"/>
@@ -1983,7 +2029,7 @@
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1998,7 +2044,7 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="O38" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
@@ -2015,7 +2061,7 @@
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -2028,11 +2074,9 @@
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
-      <c r="M39" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="M39" s="3"/>
       <c r="O39" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="P39" s="3"/>
       <c r="Q39" s="3"/>
@@ -2045,33 +2089,106 @@
       <c r="X39" s="3"/>
       <c r="Y39" s="3"/>
       <c r="Z39" s="3"/>
-      <c r="AA39" s="5" t="s">
+      <c r="AA39" s="3"/>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="O40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="3"/>
+      <c r="T40" s="3"/>
+      <c r="U40" s="3"/>
+      <c r="V40" s="3"/>
+      <c r="W40" s="3"/>
+      <c r="X40" s="3"/>
+      <c r="Y40" s="3"/>
+      <c r="Z40" s="3"/>
+      <c r="AA40" s="3"/>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
+      <c r="O41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="3"/>
+      <c r="T41" s="3"/>
+      <c r="U41" s="3"/>
+      <c r="V41" s="3"/>
+      <c r="W41" s="3"/>
+      <c r="X41" s="3"/>
+      <c r="Y41" s="3"/>
+      <c r="Z41" s="3"/>
+      <c r="AA41" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="22">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:AA14"/>
+    <mergeCell ref="C15:AA15"/>
     <mergeCell ref="C16:AA16"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="L3:AA10"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="D10:K12"/>
+    <mergeCell ref="M3:AA12"/>
+    <mergeCell ref="C18:AA18"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:J10"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C6:G6"/>
@@ -2080,13 +2197,7 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:AA13"/>
-    <mergeCell ref="C14:AA14"/>
-    <mergeCell ref="C15:AA15"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="C17:AA17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Q and modified submission sheet
</commit_message>
<xml_diff>
--- a/docs/IMR-AmpliconSubmissionSheet(your_last_name_here).xlsx
+++ b/docs/IMR-AmpliconSubmissionSheet(your_last_name_here).xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="60">
   <si>
     <t xml:space="preserve">Plate 1 </t>
   </si>
@@ -252,9 +252,6 @@
     </r>
   </si>
   <si>
-    <t>Integrated Microbiome Resource (IMR) Submission Template v.4 (Nov 2015)</t>
-  </si>
-  <si>
     <t>for our Academic Reporting:</t>
   </si>
   <si>
@@ -267,16 +264,10 @@
     <t>Sequencing target(s):</t>
   </si>
   <si>
-    <t>16S BACTERIA</t>
-  </si>
-  <si>
-    <t>16S ARCHAEA</t>
-  </si>
-  <si>
-    <t>18S EUKARYOTES</t>
-  </si>
-  <si>
     <t>OTHER</t>
+  </si>
+  <si>
+    <t>You may copy the above layout (row/column names) to add additional plates here below if needed…</t>
   </si>
   <si>
     <r>
@@ -301,11 +292,26 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> If submitting for multiple domains (16S+18S) or Archaea, send 10 uL ea.</t>
+      <t xml:space="preserve"> If submitting for multiple domains (ex: 16S+18S) or Archaea, send 10 uL ea.</t>
     </r>
   </si>
   <si>
-    <t>You may copy the above layout (row/column names) to add additional plates here below if needed…</t>
+    <t>16S BACTERIA - V6-V8</t>
+  </si>
+  <si>
+    <t>16S BACTERIA - V4</t>
+  </si>
+  <si>
+    <t>16S ARCHAEA - V6-V8</t>
+  </si>
+  <si>
+    <t>18S EUKARYOTES - V4</t>
+  </si>
+  <si>
+    <t>ITS FUNGI</t>
+  </si>
+  <si>
+    <t>Integrated Microbiome Resource (IMR) Submission Template v.5 (Feb 2016)</t>
   </si>
 </sst>
 </file>
@@ -581,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -647,12 +653,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -665,9 +683,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -697,18 +712,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1022,7 +1025,7 @@
   <dimension ref="A1:AF54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,30 +1034,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="V1" s="36" t="s">
+      <c r="A1" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="V1" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="36"/>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="33" t="s">
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="35"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="38"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="S2" s="7"/>
@@ -1073,20 +1076,20 @@
       <c r="AF2" s="7"/>
     </row>
     <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42"/>
-      <c r="J3" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="27"/>
+      <c r="J3" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
       <c r="M3" s="19"/>
       <c r="N3" s="19"/>
       <c r="O3" s="19"/>
@@ -1109,20 +1112,20 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="42"/>
-      <c r="J4" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="27"/>
+      <c r="J4" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
       <c r="M4" s="19"/>
       <c r="N4" s="19"/>
       <c r="O4" s="19"/>
@@ -1146,11 +1149,11 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I5"/>
-      <c r="J5" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
+      <c r="J5" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
       <c r="M5" s="19"/>
       <c r="N5" s="19"/>
       <c r="O5" s="19"/>
@@ -1173,15 +1176,15 @@
       <c r="AF5" s="7"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="42"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
       <c r="M6" s="19"/>
       <c r="N6" s="19"/>
       <c r="O6" s="19"/>
@@ -1204,15 +1207,15 @@
       <c r="AF6" s="7"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="42"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="27"/>
       <c r="M7" s="19"/>
       <c r="N7" s="19"/>
       <c r="O7" s="19"/>
@@ -1271,16 +1274,16 @@
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="C9" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="20" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F9" s="17"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="20" t="s">
-        <v>54</v>
+      <c r="H9" s="22"/>
+      <c r="I9" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
@@ -1312,12 +1315,12 @@
       <c r="C10" s="17"/>
       <c r="D10" s="21"/>
       <c r="E10" s="20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F10" s="17"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="20" t="s">
-        <v>55</v>
+      <c r="H10" s="22"/>
+      <c r="I10" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
@@ -1347,12 +1350,16 @@
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="20" t="s">
+        <v>56</v>
+      </c>
       <c r="F11" s="17"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="18"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="20" t="s">
+        <v>51</v>
+      </c>
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
@@ -1400,164 +1407,164 @@
       <c r="AF12" s="7"/>
     </row>
     <row r="13" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="38"/>
-      <c r="O13" s="38"/>
-      <c r="P13" s="38"/>
-      <c r="Q13" s="38"/>
-      <c r="R13" s="38"/>
-      <c r="S13" s="38"/>
-      <c r="T13" s="38"/>
-      <c r="U13" s="38"/>
-      <c r="V13" s="38"/>
-      <c r="W13" s="38"/>
-      <c r="X13" s="38"/>
-      <c r="Y13" s="38"/>
-      <c r="Z13" s="38"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="41"/>
+      <c r="Y13" s="41"/>
+      <c r="Z13" s="41"/>
       <c r="AA13" s="18"/>
     </row>
     <row r="14" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="30" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="31"/>
-      <c r="P15" s="31"/>
-      <c r="Q15" s="31"/>
-      <c r="R15" s="31"/>
-      <c r="S15" s="31"/>
-      <c r="T15" s="31"/>
-      <c r="U15" s="31"/>
-      <c r="V15" s="31"/>
-      <c r="W15" s="31"/>
-      <c r="X15" s="31"/>
-      <c r="Y15" s="31"/>
-      <c r="Z15" s="31"/>
-      <c r="AA15" s="32"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="34"/>
+      <c r="S15" s="34"/>
+      <c r="T15" s="34"/>
+      <c r="U15" s="34"/>
+      <c r="V15" s="34"/>
+      <c r="W15" s="34"/>
+      <c r="X15" s="34"/>
+      <c r="Y15" s="34"/>
+      <c r="Z15" s="34"/>
+      <c r="AA15" s="35"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="26"/>
-      <c r="S16" s="26"/>
-      <c r="T16" s="26"/>
-      <c r="U16" s="26"/>
-      <c r="V16" s="26"/>
-      <c r="W16" s="26"/>
-      <c r="X16" s="26"/>
-      <c r="Y16" s="26"/>
-      <c r="Z16" s="26"/>
-      <c r="AA16" s="27"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="30"/>
+      <c r="U16" s="30"/>
+      <c r="V16" s="30"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="30"/>
+      <c r="Y16" s="30"/>
+      <c r="Z16" s="30"/>
+      <c r="AA16" s="31"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="26"/>
-      <c r="S17" s="26"/>
-      <c r="T17" s="26"/>
-      <c r="U17" s="26"/>
-      <c r="V17" s="26"/>
-      <c r="W17" s="26"/>
-      <c r="X17" s="26"/>
-      <c r="Y17" s="26"/>
-      <c r="Z17" s="26"/>
-      <c r="AA17" s="27"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="30"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="30"/>
+      <c r="T17" s="30"/>
+      <c r="U17" s="30"/>
+      <c r="V17" s="30"/>
+      <c r="W17" s="30"/>
+      <c r="X17" s="30"/>
+      <c r="Y17" s="30"/>
+      <c r="Z17" s="30"/>
+      <c r="AA17" s="31"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
-      <c r="Q18" s="26"/>
-      <c r="R18" s="26"/>
-      <c r="S18" s="26"/>
-      <c r="T18" s="26"/>
-      <c r="U18" s="26"/>
-      <c r="V18" s="26"/>
-      <c r="W18" s="26"/>
-      <c r="X18" s="26"/>
-      <c r="Y18" s="26"/>
-      <c r="Z18" s="26"/>
-      <c r="AA18" s="27"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="30"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="30"/>
+      <c r="U18" s="30"/>
+      <c r="V18" s="30"/>
+      <c r="W18" s="30"/>
+      <c r="X18" s="30"/>
+      <c r="Y18" s="30"/>
+      <c r="Z18" s="30"/>
+      <c r="AA18" s="31"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
@@ -2415,8 +2422,8 @@
       </c>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A46" s="43" t="s">
-        <v>57</v>
+      <c r="A46" s="24" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -2436,11 +2443,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
     <mergeCell ref="C18:AA18"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A15:B15"/>
@@ -2457,6 +2459,11 @@
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C6:G6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>